<commit_message>
14TranslationRelative working with Excell file
</commit_message>
<xml_diff>
--- a/RevitDynamo/11files/relative_values.xlsx
+++ b/RevitDynamo/11files/relative_values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmsil\Desktop\bsp3\RevitDynamo\11files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16932FD-09BB-4010-B16B-7B08C55769AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAF209E-FA40-451E-9404-6005585CAD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A7A23B64-5B2A-4164-A763-E7FBE671D2B7}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="26430" windowHeight="15345" xr2:uid="{A7A23B64-5B2A-4164-A763-E7FBE671D2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Wall" sheetId="6" r:id="rId1"/>
@@ -518,7 +518,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,10 +623,10 @@
         <v>58</v>
       </c>
       <c r="P2">
-        <v>2.2999999999999998</v>
+        <v>-200</v>
       </c>
       <c r="Q2">
-        <v>-2.2999999999999998</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>